<commit_message>
ran all index experiments. need just to run fx, commodity and crypto experiments
</commit_message>
<xml_diff>
--- a/Future direction.xlsx
+++ b/Future direction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\topco\Dokumenti\MSc Banking and Digital Finance UCL\Modules\Dissertation\MSc_dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834196BC-BBCB-49C7-A82D-A3B66E923F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B5899C-C74E-4CEF-BC40-3E0253E2E510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="10500" windowWidth="25800" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1965" yWindow="2445" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments already ran" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
   <si>
     <t xml:space="preserve">Experiments </t>
   </si>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:G24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,14 +698,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>5</v>
@@ -730,12 +722,6 @@
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>15</v>
-      </c>
-      <c r="F34" t="s">
-        <v>4</v>
-      </c>
-      <c r="G34" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
just need to experiment with two types of credit card data
</commit_message>
<xml_diff>
--- a/Future direction.xlsx
+++ b/Future direction.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\topco\Dokumenti\MSc Banking and Digital Finance UCL\Modules\Dissertation\MSc_dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B5899C-C74E-4CEF-BC40-3E0253E2E510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877B5974-CE97-4345-B5B6-6E7777ACFF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1965" yWindow="2445" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8715" yWindow="1965" windowWidth="12630" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments already ran" sheetId="1" r:id="rId1"/>
     <sheet name="Future experiments" sheetId="2" r:id="rId2"/>
+    <sheet name="questions for Ramin" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
   <si>
     <t xml:space="preserve">Experiments </t>
   </si>
@@ -158,6 +159,12 @@
   </si>
   <si>
     <t>focus of TSFM vs benchmark comparison (as before)</t>
+  </si>
+  <si>
+    <t>Into how much detail should I go in the background section where I talk about the models?</t>
+  </si>
+  <si>
+    <t>What about the Code? Does code have to be really clean? Should code be explained? Is this something that I will be graded on?</t>
   </si>
 </sst>
 </file>
@@ -484,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,54 +670,86 @@
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F23" t="s">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F24" t="s">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G24" t="s">
-        <v>17</v>
-      </c>
+      <c r="G24" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E27" t="s">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -741,7 +780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0EF2138-4500-4BB0-8C60-7FFA97BC9B82}">
   <dimension ref="B2:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -907,4 +946,29 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7952DB6-F2CE-4570-9F3B-5A1ADB5F6646}">
+  <dimension ref="D5:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>